<commit_message>
Update students data in Excel format
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhase\OneDrive\Documents\Jacob\Programing\AIEducation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7E24E9-7314-4AA3-9E5C-0D922C369D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC28F9D-320E-4ED0-9FC0-4995CC189C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,14 +157,14 @@
     <t>Advanced</t>
   </si>
   <si>
-    <t>students.xlsx</t>
+    <t>Student ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,12 +179,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF6A9955"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,13 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,12 +527,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>